<commit_message>
Fix Silent-Validate-PreReq.aip - hide APPDIR by setting it to C:\ProgramData\RISA; also mention Loud and Silent.aip test project in documentation
</commit_message>
<xml_diff>
--- a/Documentation/Integrating Silent Install into AI Installers.xlsx
+++ b/Documentation/Integrating Silent Install into AI Installers.xlsx
@@ -5,12 +5,12 @@
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\aaKE\ProjDocs\DBs\SW\RISA-Adv Installer impl\035-Silent Install\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Advanced Installer\Documentation\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{465ADA5A-6780-4767-8D35-149CA4C94209}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{3B29C256-1E3F-4373-8BC6-3280A8AF5410}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-23004" yWindow="6492" windowWidth="20412" windowHeight="18324" activeTab="5" xr2:uid="{757481C7-A015-4B07-931A-B1A835412FCC}"/>
+    <workbookView xWindow="-22512" yWindow="5736" windowWidth="19932" windowHeight="14304" firstSheet="1" activeTab="1" xr2:uid="{757481C7-A015-4B07-931A-B1A835412FCC}"/>
   </bookViews>
   <sheets>
     <sheet name="SI-RoadMap" sheetId="2" r:id="rId1"/>
@@ -38,7 +38,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="78" uniqueCount="78">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="81" uniqueCount="81">
   <si>
     <t>Installer Phases for Loud and Silent Install - how the parts fit together</t>
   </si>
@@ -272,6 +272,15 @@
   </si>
   <si>
     <t>using setup.ini in same dir as installer, it should find it</t>
+  </si>
+  <si>
+    <t>Sample project that integrates Silent Install:</t>
+  </si>
+  <si>
+    <t>C:\Advanced Installer\Projects\Common\Custom Actions\CA-Test-Installers</t>
+  </si>
+  <si>
+    <t>3D-1901-Loud-and-Silent.aip</t>
   </si>
 </sst>
 </file>
@@ -1448,10 +1457,10 @@
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{50A413C1-57A0-4EC0-BC26-8BFE81F213C0}">
-  <dimension ref="B3:N15"/>
+  <dimension ref="B3:N20"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="D68" sqref="D68"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="R15" sqref="R15"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="7" defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
@@ -1492,6 +1501,21 @@
     <row r="15" spans="2:14" x14ac:dyDescent="0.3">
       <c r="M15" s="1" t="s">
         <v>10</v>
+      </c>
+    </row>
+    <row r="18" spans="11:13" x14ac:dyDescent="0.3">
+      <c r="K18" s="1" t="s">
+        <v>78</v>
+      </c>
+    </row>
+    <row r="19" spans="11:13" x14ac:dyDescent="0.3">
+      <c r="L19" s="1" t="s">
+        <v>79</v>
+      </c>
+    </row>
+    <row r="20" spans="11:13" x14ac:dyDescent="0.3">
+      <c r="M20" s="1" t="s">
+        <v>80</v>
       </c>
     </row>
   </sheetData>
@@ -1759,8 +1783,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{88F24209-EBF6-4647-B3A0-447F35841C49}">
   <dimension ref="B2:L26"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="S6" sqref="S6"/>
+    <sheetView workbookViewId="0">
+      <selection activeCell="A3" sqref="A3:XFD3"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="6.77734375" defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>

</xml_diff>